<commit_message>
move agr, waste, forestry activity formulas to prov activity file
</commit_message>
<xml_diff>
--- a/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
+++ b/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\sector_forestry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42A25D68-A964-4844-B767-B920435E91F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62E9E6BE-4C8B-413D-8ED1-06B29893801D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85879F7-9531-4B82-83C2-39468D892AD5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5644D5BA-9F23-402B-8A6B-35AE71ACC625}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -247,6 +250,82 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="BC"/>
+      <sheetName val="AB"/>
+      <sheetName val="SK"/>
+      <sheetName val="MB"/>
+      <sheetName val="ON"/>
+      <sheetName val="QC"/>
+      <sheetName val="NB"/>
+      <sheetName val="NS"/>
+      <sheetName val="PE"/>
+      <sheetName val="NL"/>
+      <sheetName val="YT"/>
+      <sheetName val="NT"/>
+      <sheetName val="NU"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="100">
+          <cell r="E100">
+            <v>1000000</v>
+          </cell>
+          <cell r="F100">
+            <v>1300000</v>
+          </cell>
+          <cell r="G100">
+            <v>700000</v>
+          </cell>
+          <cell r="H100">
+            <v>1000000</v>
+          </cell>
+          <cell r="I100">
+            <v>1100000</v>
+          </cell>
+          <cell r="J100">
+            <v>1100000</v>
+          </cell>
+          <cell r="K100">
+            <v>1100000</v>
+          </cell>
+          <cell r="L100">
+            <v>1100000</v>
+          </cell>
+          <cell r="M100">
+            <v>1100000</v>
+          </cell>
+          <cell r="N100">
+            <v>1100000</v>
+          </cell>
+          <cell r="O100">
+            <v>1100000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -565,7 +644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C7016E-62FE-4DA5-8611-8B60689716FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73FD37B-994E-48FF-814A-D053BFB157BD}">
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -676,47 +755,47 @@
         <v>19</v>
       </c>
       <c r="M3">
-        <f>1000000*1</f>
+        <f>[1]BC!E$100</f>
         <v>1000000</v>
       </c>
       <c r="N3">
-        <f>1000000*1.3</f>
+        <f>[1]BC!F$100</f>
         <v>1300000</v>
       </c>
       <c r="O3">
-        <f>1000000*0.7</f>
+        <f>[1]BC!G$100</f>
         <v>700000</v>
       </c>
       <c r="P3">
-        <f>1000000*1</f>
+        <f>[1]BC!H$100</f>
         <v>1000000</v>
       </c>
       <c r="Q3">
-        <f>1000000*1.1</f>
+        <f>[1]BC!I$100</f>
         <v>1100000</v>
       </c>
       <c r="R3">
-        <f>Q3</f>
+        <f>[1]BC!J$100</f>
         <v>1100000</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:W3" si="0">R3</f>
+        <f>[1]BC!K$100</f>
         <v>1100000</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
+        <f>[1]BC!L$100</f>
         <v>1100000</v>
       </c>
       <c r="U3">
-        <f t="shared" si="0"/>
+        <f>[1]BC!M$100</f>
         <v>1100000</v>
       </c>
       <c r="V3">
-        <f t="shared" si="0"/>
+        <f>[1]BC!N$100</f>
         <v>1100000</v>
       </c>
       <c r="W3">
-        <f t="shared" si="0"/>
+        <f>[1]BC!O$100</f>
         <v>1100000</v>
       </c>
     </row>
@@ -1964,39 +2043,39 @@
         <v>1</v>
       </c>
       <c r="O26">
-        <f t="shared" ref="O26:W26" si="1">N26</f>
+        <f t="shared" ref="O26:W26" si="0">N26</f>
         <v>1</v>
       </c>
       <c r="P26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="S26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="T26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="V26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="W26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2131,43 +2210,43 @@
         <v>14.237915569160673</v>
       </c>
       <c r="N31">
-        <f t="shared" ref="N31:W31" si="2">M31</f>
+        <f t="shared" ref="N31:W31" si="1">M31</f>
         <v>14.237915569160673</v>
       </c>
       <c r="O31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="P31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="R31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="S31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="T31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="U31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="V31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
       <c r="W31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move BC temporary files to repository files
</commit_message>
<xml_diff>
--- a/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
+++ b/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\sector_forestry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62E9E6BE-4C8B-413D-8ED1-06B29893801D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2573F48A-D70C-4691-B386-6D60F0FEDE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5644D5BA-9F23-402B-8A6B-35AE71ACC625}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EDFF35DB-F5B4-43E7-8E6E-C826EF314EBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="57">
+  <si>
+    <t>CIMS.CAN.BC.Light Industrial.Water Heating</t>
+  </si>
   <si>
     <t>&lt;-- Navigate by typing to search</t>
   </si>
@@ -197,7 +200,16 @@
     <t>%</t>
   </si>
   <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
     <t>GJ</t>
+  </si>
+  <si>
+    <t>Electric</t>
   </si>
 </sst>
 </file>
@@ -259,6 +271,7 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
+      <sheetName val="CAN"/>
       <sheetName val="BC"/>
       <sheetName val="AB"/>
       <sheetName val="SK"/>
@@ -274,44 +287,44 @@
       <sheetName val="NU"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="100">
-          <cell r="E100">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="103">
+          <cell r="E103">
             <v>1000000</v>
           </cell>
-          <cell r="F100">
+          <cell r="F103">
             <v>1300000</v>
           </cell>
-          <cell r="G100">
+          <cell r="G103">
             <v>700000</v>
           </cell>
-          <cell r="H100">
+          <cell r="H103">
             <v>1000000</v>
           </cell>
-          <cell r="I100">
+          <cell r="I103">
             <v>1100000</v>
           </cell>
-          <cell r="J100">
+          <cell r="J103">
             <v>1100000</v>
           </cell>
-          <cell r="K100">
+          <cell r="K103">
             <v>1100000</v>
           </cell>
-          <cell r="L100">
+          <cell r="L103">
             <v>1100000</v>
           </cell>
-          <cell r="M100">
+          <cell r="M103">
             <v>1100000</v>
           </cell>
-          <cell r="N100">
+          <cell r="N103">
             <v>1100000</v>
           </cell>
-          <cell r="O100">
+          <cell r="O103">
             <v>1100000</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
@@ -323,6 +336,7 @@
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -644,56 +658,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73FD37B-994E-48FF-814A-D053BFB157BD}">
-  <dimension ref="A1:X31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6FC1FD-06C1-43ED-9AC9-38D64B57354C}">
+  <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X31"/>
+      <selection sqref="A1:X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -729,131 +746,131 @@
         <v>2050</v>
       </c>
       <c r="X2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3">
-        <f>[1]BC!E$100</f>
+        <f>[1]BC!E$103</f>
         <v>1000000</v>
       </c>
       <c r="N3">
-        <f>[1]BC!F$100</f>
+        <f>[1]BC!F$103</f>
         <v>1300000</v>
       </c>
       <c r="O3">
-        <f>[1]BC!G$100</f>
+        <f>[1]BC!G$103</f>
         <v>700000</v>
       </c>
       <c r="P3">
-        <f>[1]BC!H$100</f>
+        <f>[1]BC!H$103</f>
         <v>1000000</v>
       </c>
       <c r="Q3">
-        <f>[1]BC!I$100</f>
+        <f>[1]BC!I$103</f>
         <v>1100000</v>
       </c>
       <c r="R3">
-        <f>[1]BC!J$100</f>
+        <f>[1]BC!J$103</f>
         <v>1100000</v>
       </c>
       <c r="S3">
-        <f>[1]BC!K$100</f>
+        <f>[1]BC!K$103</f>
         <v>1100000</v>
       </c>
       <c r="T3">
-        <f>[1]BC!L$100</f>
+        <f>[1]BC!L$103</f>
         <v>1100000</v>
       </c>
       <c r="U3">
-        <f>[1]BC!M$100</f>
+        <f>[1]BC!M$103</f>
         <v>1100000</v>
       </c>
       <c r="V3">
-        <f>[1]BC!N$100</f>
+        <f>[1]BC!N$103</f>
         <v>1100000</v>
       </c>
       <c r="W3">
-        <f>[1]BC!O$100</f>
+        <f>[1]BC!O$103</f>
         <v>1100000</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
         <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M6">
         <v>1.1853107044796758</v>
@@ -889,89 +906,89 @@
         <v>2.528656305562841</v>
       </c>
       <c r="X6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
         <v>26</v>
-      </c>
-      <c r="K7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1007,30 +1024,30 @@
         <v>1</v>
       </c>
       <c r="X8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -1066,30 +1083,30 @@
         <v>1</v>
       </c>
       <c r="X9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -1125,30 +1142,30 @@
         <v>1</v>
       </c>
       <c r="X10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M11">
         <v>0.52061381217929492</v>
@@ -1184,30 +1201,30 @@
         <v>1.4405383838732864</v>
       </c>
       <c r="X11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M12">
         <v>1.67</v>
@@ -1243,30 +1260,30 @@
         <v>1.67</v>
       </c>
       <c r="X12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -1302,30 +1319,30 @@
         <v>1</v>
       </c>
       <c r="X13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M14">
         <v>1.0160053775773112</v>
@@ -1361,30 +1378,30 @@
         <v>0.96565680121894615</v>
       </c>
       <c r="X14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -1420,30 +1437,30 @@
         <v>1</v>
       </c>
       <c r="X15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M16">
         <v>0.99999999982762755</v>
@@ -1479,30 +1496,30 @@
         <v>0.99999999992841759</v>
       </c>
       <c r="X16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -1538,30 +1555,30 @@
         <v>1</v>
       </c>
       <c r="X17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -1597,30 +1614,30 @@
         <v>1</v>
       </c>
       <c r="X18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M19">
         <v>1.0557392141561774</v>
@@ -1656,30 +1673,30 @@
         <v>0.84547528189865873</v>
       </c>
       <c r="X19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -1715,30 +1732,30 @@
         <v>1</v>
       </c>
       <c r="X20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -1774,30 +1791,30 @@
         <v>1</v>
       </c>
       <c r="X21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -1833,30 +1850,30 @@
         <v>1</v>
       </c>
       <c r="X22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1892,30 +1909,30 @@
         <v>1</v>
       </c>
       <c r="X23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -1951,30 +1968,30 @@
         <v>1</v>
       </c>
       <c r="X24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -2010,30 +2027,30 @@
         <v>1</v>
       </c>
       <c r="X25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" t="s">
-        <v>17</v>
-      </c>
       <c r="J26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -2081,97 +2098,97 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" t="s">
         <v>20</v>
-      </c>
-      <c r="L27" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -2179,74 +2196,337 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M31">
+        <v>20</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ref="N31:W32" si="1">M31</f>
+        <v>20</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="F31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" t="s">
-        <v>30</v>
-      </c>
-      <c r="L31" t="s">
-        <v>52</v>
-      </c>
-      <c r="M31">
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" t="s">
+        <v>55</v>
+      </c>
+      <c r="M32">
         <f>1/0.070235</f>
         <v>14.237915569160673</v>
       </c>
-      <c r="N31">
-        <f t="shared" ref="N31:W31" si="1">M31</f>
-        <v>14.237915569160673</v>
-      </c>
-      <c r="O31">
+      <c r="N32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="P31">
+      <c r="O32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="Q31">
+      <c r="P32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="R31">
+      <c r="Q32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="S31">
+      <c r="R32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="T31">
+      <c r="S32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="U31">
+      <c r="T32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="V31">
+      <c r="U32">
         <f t="shared" si="1"/>
         <v>14.237915569160673</v>
       </c>
-      <c r="W31">
+      <c r="V32">
         <f t="shared" si="1"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="1"/>
+        <v>14.237915569160673</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34" t="s">
+        <v>52</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" t="s">
+        <v>53</v>
+      </c>
+      <c r="L35" t="s">
+        <v>54</v>
+      </c>
+      <c r="M35">
+        <v>20</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ref="N35:W36" si="2">M35</f>
+        <v>20</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L36" t="s">
+        <v>55</v>
+      </c>
+      <c r="M36">
+        <f>1/0.070235</f>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="2"/>
+        <v>14.237915569160673</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="2"/>
         <v>14.237915569160673</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move electricity price multipliers from exog_prices to sector files
</commit_message>
<xml_diff>
--- a/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
+++ b/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\sector_forestry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2573F48A-D70C-4691-B386-6D60F0FEDE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A807F361-7856-4C6D-8E0E-2B28286B6CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EDFF35DB-F5B4-43E7-8E6E-C826EF314EBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD72D202-3702-42D2-BDB6-BA729C6F68E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="57">
-  <si>
-    <t>CIMS.CAN.BC.Light Industrial.Water Heating</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="56">
   <si>
     <t>&lt;-- Navigate by typing to search</t>
   </si>
@@ -658,7 +655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6FC1FD-06C1-43ED-9AC9-38D64B57354C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6A09D5-1C1C-4B2D-9A8F-67854D65FEFF}">
   <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -668,49 +665,46 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -746,30 +740,30 @@
         <v>2050</v>
       </c>
       <c r="X2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
       </c>
       <c r="M3">
         <f>[1]BC!E$103</f>
@@ -818,59 +812,65 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>24</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
       </c>
       <c r="M6">
         <v>1.1853107044796758</v>
@@ -906,266 +906,266 @@
         <v>2.528656305562841</v>
       </c>
       <c r="X6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
         <v>25</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8" t="s">
         <v>25</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9" t="s">
         <v>25</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="W9">
-        <v>1</v>
-      </c>
-      <c r="X9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10" t="s">
         <v>25</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
-      <c r="W10">
-        <v>1</v>
-      </c>
-      <c r="X10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M11">
         <v>0.52061381217929492</v>
@@ -1201,30 +1201,30 @@
         <v>1.4405383838732864</v>
       </c>
       <c r="X11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" t="s">
         <v>32</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
       </c>
       <c r="M12">
         <v>1.67</v>
@@ -1260,89 +1260,89 @@
         <v>1.67</v>
       </c>
       <c r="X12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13" t="s">
         <v>25</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="S13">
-        <v>1</v>
-      </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-      <c r="V13">
-        <v>1</v>
-      </c>
-      <c r="W13">
-        <v>1</v>
-      </c>
-      <c r="X13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M14">
         <v>1.0160053775773112</v>
@@ -1378,89 +1378,89 @@
         <v>0.96565680121894615</v>
       </c>
       <c r="X14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15" t="s">
         <v>25</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M16">
         <v>0.99999999982762755</v>
@@ -1496,148 +1496,148 @@
         <v>0.99999999992841759</v>
       </c>
       <c r="X16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17" t="s">
         <v>25</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17">
-        <v>1</v>
-      </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
-      <c r="W17">
-        <v>1</v>
-      </c>
-      <c r="X17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18" t="s">
         <v>25</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
-      <c r="V18">
-        <v>1</v>
-      </c>
-      <c r="W18">
-        <v>1</v>
-      </c>
-      <c r="X18" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M19">
         <v>1.0557392141561774</v>
@@ -1673,384 +1673,384 @@
         <v>0.84547528189865873</v>
       </c>
       <c r="X19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20" t="s">
         <v>25</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="T20">
-        <v>1</v>
-      </c>
-      <c r="U20">
-        <v>1</v>
-      </c>
-      <c r="V20">
-        <v>1</v>
-      </c>
-      <c r="W20">
-        <v>1</v>
-      </c>
-      <c r="X20" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21" t="s">
         <v>25</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21">
-        <v>1</v>
-      </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
-      <c r="V21">
-        <v>1</v>
-      </c>
-      <c r="W21">
-        <v>1</v>
-      </c>
-      <c r="X21" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K22" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22" t="s">
         <v>25</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
-      <c r="T22">
-        <v>1</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22">
-        <v>1</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
-      <c r="X22" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23" t="s">
         <v>25</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-      <c r="T23">
-        <v>1</v>
-      </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
-      <c r="V23">
-        <v>1</v>
-      </c>
-      <c r="W23">
-        <v>1</v>
-      </c>
-      <c r="X23" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K24" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24" t="s">
         <v>25</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-      <c r="S24">
-        <v>1</v>
-      </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
-      <c r="U24">
-        <v>1</v>
-      </c>
-      <c r="V24">
-        <v>1</v>
-      </c>
-      <c r="W24">
-        <v>1</v>
-      </c>
-      <c r="X24" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K25" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25" t="s">
         <v>25</v>
-      </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
-      <c r="T25">
-        <v>1</v>
-      </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-      <c r="V25">
-        <v>1</v>
-      </c>
-      <c r="W25">
-        <v>1</v>
-      </c>
-      <c r="X25" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26" t="s">
         <v>19</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" t="s">
-        <v>47</v>
-      </c>
-      <c r="L26" t="s">
-        <v>20</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -2098,97 +2098,97 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
         <v>47</v>
       </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" t="s">
-        <v>48</v>
-      </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
         <v>47</v>
       </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" t="s">
         <v>48</v>
-      </c>
-      <c r="G28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
+      <c r="F29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" t="s">
         <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
         <v>47</v>
       </c>
-      <c r="B30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" t="s">
-        <v>48</v>
-      </c>
       <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s">
         <v>50</v>
       </c>
-      <c r="G30" t="s">
+      <c r="L30" t="s">
         <v>51</v>
-      </c>
-      <c r="L30" t="s">
-        <v>52</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -2196,28 +2196,28 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
         <v>47</v>
       </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="s">
-        <v>48</v>
-      </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G31" t="s">
+        <v>52</v>
+      </c>
+      <c r="L31" t="s">
         <v>53</v>
-      </c>
-      <c r="L31" t="s">
-        <v>54</v>
       </c>
       <c r="M31">
         <v>20</v>
@@ -2265,31 +2265,31 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
         <v>47</v>
       </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="E32" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" t="s">
-        <v>18</v>
-      </c>
       <c r="J32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M32">
         <f>1/0.070235</f>
@@ -2338,51 +2338,51 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
         <v>47</v>
       </c>
-      <c r="B33" t="s">
+      <c r="F33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" t="s">
         <v>6</v>
-      </c>
-      <c r="C33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" t="s">
-        <v>56</v>
-      </c>
-      <c r="G33" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
         <v>47</v>
       </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" t="s">
-        <v>48</v>
-      </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" t="s">
         <v>51</v>
-      </c>
-      <c r="L34" t="s">
-        <v>52</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -2390,28 +2390,28 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
         <v>47</v>
       </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
-        <v>48</v>
-      </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G35" t="s">
+        <v>52</v>
+      </c>
+      <c r="L35" t="s">
         <v>53</v>
-      </c>
-      <c r="L35" t="s">
-        <v>54</v>
       </c>
       <c r="M35">
         <v>20</v>
@@ -2459,31 +2459,31 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
         <v>47</v>
       </c>
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" t="s">
         <v>17</v>
       </c>
-      <c r="E36" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" t="s">
-        <v>56</v>
-      </c>
-      <c r="G36" t="s">
-        <v>18</v>
-      </c>
       <c r="J36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M36">
         <f>1/0.070235</f>

</xml_diff>

<commit_message>
Latest changes to model and policy files from EMH national modelling. Updates to csv editor and results viewer. Jupyter notebooks for Reference and Net Zero.
</commit_message>
<xml_diff>
--- a/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
+++ b/csv/model/sector_forestry/formula_sector_forestry_BC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\sector_forestry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A807F361-7856-4C6D-8E0E-2B28286B6CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7829BE64-87D5-4BE9-967B-CC98BA0BA7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD72D202-3702-42D2-BDB6-BA729C6F68E3}"/>
+    <workbookView xWindow="28680" yWindow="-1800" windowWidth="51840" windowHeight="21120" xr2:uid="{DBBF9C38-A599-45EE-8FDA-1189984B1998}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="57">
   <si>
     <t>&lt;-- Navigate by typing to search</t>
   </si>
@@ -201,6 +223,9 @@
   </si>
   <si>
     <t>Years</t>
+  </si>
+  <si>
+    <t>CIMS.CAN.BC.Fuel Blends.Diesel_Transportation</t>
   </si>
   <si>
     <t>GJ</t>
@@ -268,60 +293,56 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="CAN"/>
-      <sheetName val="BC"/>
-      <sheetName val="AB"/>
-      <sheetName val="SK"/>
-      <sheetName val="MB"/>
-      <sheetName val="ON"/>
-      <sheetName val="QC"/>
-      <sheetName val="NB"/>
-      <sheetName val="NS"/>
-      <sheetName val="PE"/>
-      <sheetName val="NL"/>
-      <sheetName val="YT"/>
-      <sheetName val="NT"/>
-      <sheetName val="NU"/>
+      <sheetName val="CAN_0"/>
+      <sheetName val="BC_0"/>
+      <sheetName val="AB_0"/>
+      <sheetName val="SK_0"/>
+      <sheetName val="MB_0"/>
+      <sheetName val="ON_0"/>
+      <sheetName val="QC_0"/>
+      <sheetName val="NB_0"/>
+      <sheetName val="NS_0"/>
+      <sheetName val="PE_0"/>
+      <sheetName val="NL_0"/>
+      <sheetName val="YT_0"/>
+      <sheetName val="NT_0"/>
+      <sheetName val="NU_0"/>
+      <sheetName val="Solver"/>
+      <sheetName val="Residual_1"/>
+      <sheetName val="BC_1"/>
+      <sheetName val="AB_1"/>
+      <sheetName val="ON_1"/>
+      <sheetName val="QC_1"/>
+      <sheetName val="SK_1"/>
+      <sheetName val="MB_1"/>
+      <sheetName val="NB_1"/>
+      <sheetName val="NS_1"/>
+      <sheetName val="PE_1"/>
+      <sheetName val="NL_1"/>
+      <sheetName val="YT_1"/>
+      <sheetName val="NT_1"/>
+      <sheetName val="NU_1"/>
+      <sheetName val="Residual_2"/>
+      <sheetName val="BC_2"/>
+      <sheetName val="AB_2"/>
+      <sheetName val="SK_2"/>
+      <sheetName val="MB_2"/>
+      <sheetName val="ON_2"/>
+      <sheetName val="QC_2"/>
+      <sheetName val="NB_2"/>
+      <sheetName val="NS_2"/>
+      <sheetName val="PE_2"/>
+      <sheetName val="NL_2"/>
+      <sheetName val="YT_2"/>
+      <sheetName val="NT_2"/>
+      <sheetName val="NU_2"/>
+      <sheetName val="AT_2"/>
+      <sheetName val="TR_2"/>
+      <sheetName val="Residual_3"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="103">
-          <cell r="E103">
-            <v>1000000</v>
-          </cell>
-          <cell r="F103">
-            <v>1300000</v>
-          </cell>
-          <cell r="G103">
-            <v>700000</v>
-          </cell>
-          <cell r="H103">
-            <v>1000000</v>
-          </cell>
-          <cell r="I103">
-            <v>1100000</v>
-          </cell>
-          <cell r="J103">
-            <v>1100000</v>
-          </cell>
-          <cell r="K103">
-            <v>1100000</v>
-          </cell>
-          <cell r="L103">
-            <v>1100000</v>
-          </cell>
-          <cell r="M103">
-            <v>1100000</v>
-          </cell>
-          <cell r="N103">
-            <v>1100000</v>
-          </cell>
-          <cell r="O103">
-            <v>1100000</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
@@ -334,6 +355,1359 @@
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30">
+        <row r="1">
+          <cell r="A1">
+            <v>2000</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Economic Category Total</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7" t="str">
+            <v>Mt CO2 equivalent</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Totala,b</v>
+          </cell>
+          <cell r="C8">
+            <v>63.634000000000007</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>ECONOMIC CATEGORY</v>
+          </cell>
+          <cell r="C9">
+            <v>12.215999999999999</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10">
+            <v>11.578000000000001</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>8.4120000000000008</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>0.96100000000000008</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="C13">
+            <v>0.96100000000000008</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="C15">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="C19">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20">
+            <v>2.2050000000000001</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21">
+            <v>0.63800000000000001</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22">
+            <v>0.45300000000000001</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23">
+            <v>0.185</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1.667</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>18.769000000000002</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="C26">
+            <v>11.899000000000001</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>10.038</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>1.861</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>5.5469999999999997</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30">
+            <v>4.4480000000000004</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>1.099</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32">
+            <v>1.323</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>9.3440000000000012</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>0.36799999999999999</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>2.4890000000000003</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>3.3959999999999999</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>6.9000000000000006E-2</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>1.958</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="C39">
+            <v>0.30199999999999999</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="C40">
+            <v>0.76200000000000001</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="C41">
+            <v>8.8010000000000002</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="C42">
+            <v>3.8540000000000001</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="C43">
+            <v>4.9469999999999992</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="C44">
+            <v>2.9290000000000003</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="C45">
+            <v>0.443</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="C46">
+            <v>0.13500000000000001</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="C47">
+            <v>2.351</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="C48">
+            <v>2.9709999999999996</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="C49">
+            <v>2.7499999999999996</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="C50">
+            <v>0.221</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="C51">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="C52">
+            <v>2.2709999999999999</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="C53">
+            <v>4.6660000000000013</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="C54">
+            <v>3.117</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="C55">
+            <v>0.58099999999999996</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="C56">
+            <v>0.96800000000000008</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>2005</v>
+          </cell>
+          <cell r="C60" t="str">
+            <v>Economic Category Total</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="C66" t="str">
+            <v>Mt CO2 equivalent</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>Totala,b</v>
+          </cell>
+          <cell r="C67">
+            <v>62.683</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>ECONOMIC CATEGORY</v>
+          </cell>
+          <cell r="C68">
+            <v>13.532000000000002</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="C69">
+            <v>12.895</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="C70">
+            <v>10.718999999999999</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="C71">
+            <v>0.74299999999999999</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="C72">
+            <v>0.74299999999999999</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="C73">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="C74">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="C75">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="C76">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="C77">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="C78">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="C79">
+            <v>1.4329999999999998</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="C80">
+            <v>0.63700000000000001</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="C81">
+            <v>0.53500000000000003</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="C82">
+            <v>0.10200000000000001</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="C83">
+            <v>1.0309999999999999</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="C84">
+            <v>19.53</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="C85">
+            <v>11.745000000000001</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="C86">
+            <v>9.8710000000000004</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="C87">
+            <v>1.8739999999999999</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="C88">
+            <v>6.4089999999999998</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="C89">
+            <v>5.2810000000000006</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="C90">
+            <v>1.1280000000000001</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="C91">
+            <v>1.3759999999999999</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="C92">
+            <v>7.1559999999999997</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="C93">
+            <v>0.41699999999999998</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="C94">
+            <v>1.6559999999999999</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="C95">
+            <v>1.8399999999999999</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="C96">
+            <v>5.0000000000000001E-3</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="C97">
+            <v>2.0339999999999998</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="C98">
+            <v>0.30499999999999999</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="C99">
+            <v>0.89900000000000002</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="C100">
+            <v>8.4660000000000011</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="C101">
+            <v>3.758</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="C102">
+            <v>4.7080000000000002</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="C103">
+            <v>2.8699999999999997</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="C104">
+            <v>0.218</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="C105">
+            <v>0.124</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="C106">
+            <v>2.5279999999999996</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="C107">
+            <v>2.7280000000000002</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="C108">
+            <v>2.5</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="C109">
+            <v>0.22800000000000001</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="C110">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="C111">
+            <v>2.1080000000000001</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="C112">
+            <v>5.2620000000000005</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="C113">
+            <v>3.266</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="C114">
+            <v>0.745</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="C115">
+            <v>1.2509999999999999</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119">
+            <v>2010</v>
+          </cell>
+          <cell r="C119" t="str">
+            <v>Economic Category Total</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="C125" t="str">
+            <v>Mt CO2 equivalent</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126" t="str">
+            <v>Totala,b</v>
+          </cell>
+          <cell r="C126">
+            <v>59.622</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127" t="str">
+            <v>ECONOMIC CATEGORY</v>
+          </cell>
+          <cell r="C127">
+            <v>15.360999999999999</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="C128">
+            <v>14.517999999999999</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="C129">
+            <v>12.800000000000002</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="C130">
+            <v>0.64900000000000002</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="C131">
+            <v>0.64900000000000002</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="C132">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="C133">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="C134">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="135">
+          <cell r="C135">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="136">
+          <cell r="C136">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="137">
+          <cell r="C137">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="138">
+          <cell r="C138">
+            <v>1.069</v>
+          </cell>
+        </row>
+        <row r="139">
+          <cell r="C139">
+            <v>0.84300000000000008</v>
+          </cell>
+        </row>
+        <row r="140">
+          <cell r="C140">
+            <v>0.71600000000000008</v>
+          </cell>
+        </row>
+        <row r="141">
+          <cell r="C141">
+            <v>0.127</v>
+          </cell>
+        </row>
+        <row r="142">
+          <cell r="C142">
+            <v>0.9830000000000001</v>
+          </cell>
+        </row>
+        <row r="143">
+          <cell r="C143">
+            <v>19.413999999999998</v>
+          </cell>
+        </row>
+        <row r="144">
+          <cell r="C144">
+            <v>10.955</v>
+          </cell>
+        </row>
+        <row r="145">
+          <cell r="C145">
+            <v>9.3629999999999995</v>
+          </cell>
+        </row>
+        <row r="146">
+          <cell r="C146">
+            <v>1.5920000000000001</v>
+          </cell>
+        </row>
+        <row r="147">
+          <cell r="C147">
+            <v>7.2299999999999995</v>
+          </cell>
+        </row>
+        <row r="148">
+          <cell r="C148">
+            <v>6.2709999999999999</v>
+          </cell>
+        </row>
+        <row r="149">
+          <cell r="C149">
+            <v>0.95900000000000007</v>
+          </cell>
+        </row>
+        <row r="150">
+          <cell r="C150">
+            <v>1.2290000000000001</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="C151">
+            <v>5.6659999999999995</v>
+          </cell>
+        </row>
+        <row r="152">
+          <cell r="C152">
+            <v>0.27</v>
+          </cell>
+        </row>
+        <row r="153">
+          <cell r="C153">
+            <v>1.3490000000000002</v>
+          </cell>
+        </row>
+        <row r="154">
+          <cell r="C154">
+            <v>1.9239999999999999</v>
+          </cell>
+        </row>
+        <row r="155">
+          <cell r="C155">
+            <v>3.6000000000000004E-2</v>
+          </cell>
+        </row>
+        <row r="156">
+          <cell r="C156">
+            <v>1.401</v>
+          </cell>
+        </row>
+        <row r="157">
+          <cell r="C157">
+            <v>0.23899999999999999</v>
+          </cell>
+        </row>
+        <row r="158">
+          <cell r="C158">
+            <v>0.44700000000000001</v>
+          </cell>
+        </row>
+        <row r="159">
+          <cell r="C159">
+            <v>8.1859999999999999</v>
+          </cell>
+        </row>
+        <row r="160">
+          <cell r="C160">
+            <v>3.4989999999999997</v>
+          </cell>
+        </row>
+        <row r="161">
+          <cell r="C161">
+            <v>4.6870000000000003</v>
+          </cell>
+        </row>
+        <row r="162">
+          <cell r="C162">
+            <v>2.456</v>
+          </cell>
+        </row>
+        <row r="163">
+          <cell r="C163">
+            <v>0.42399999999999999</v>
+          </cell>
+        </row>
+        <row r="164">
+          <cell r="C164">
+            <v>0.11799999999999999</v>
+          </cell>
+        </row>
+        <row r="165">
+          <cell r="C165">
+            <v>1.9140000000000001</v>
+          </cell>
+        </row>
+        <row r="166">
+          <cell r="C166">
+            <v>2.9420000000000002</v>
+          </cell>
+        </row>
+        <row r="167">
+          <cell r="C167">
+            <v>2.7</v>
+          </cell>
+        </row>
+        <row r="168">
+          <cell r="C168">
+            <v>0.24199999999999999</v>
+          </cell>
+        </row>
+        <row r="169">
+          <cell r="C169">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="170">
+          <cell r="C170">
+            <v>2.1150000000000002</v>
+          </cell>
+        </row>
+        <row r="171">
+          <cell r="C171">
+            <v>2.4989999999999997</v>
+          </cell>
+        </row>
+        <row r="172">
+          <cell r="C172">
+            <v>1.306</v>
+          </cell>
+        </row>
+        <row r="173">
+          <cell r="C173">
+            <v>0.47100000000000003</v>
+          </cell>
+        </row>
+        <row r="174">
+          <cell r="C174">
+            <v>0.72199999999999998</v>
+          </cell>
+        </row>
+        <row r="178">
+          <cell r="A178">
+            <v>2015</v>
+          </cell>
+          <cell r="C178" t="str">
+            <v>Economic Category Total</v>
+          </cell>
+        </row>
+        <row r="184">
+          <cell r="C184" t="str">
+            <v>Mt CO2 equivalent</v>
+          </cell>
+        </row>
+        <row r="185">
+          <cell r="A185" t="str">
+            <v>Totala,b</v>
+          </cell>
+          <cell r="C185">
+            <v>59.664999999999999</v>
+          </cell>
+        </row>
+        <row r="186">
+          <cell r="A186" t="str">
+            <v>ECONOMIC CATEGORY</v>
+          </cell>
+          <cell r="C186">
+            <v>15.272999999999998</v>
+          </cell>
+        </row>
+        <row r="187">
+          <cell r="C187">
+            <v>14.552</v>
+          </cell>
+        </row>
+        <row r="188">
+          <cell r="C188">
+            <v>12.414000000000001</v>
+          </cell>
+        </row>
+        <row r="189">
+          <cell r="C189">
+            <v>0.629</v>
+          </cell>
+        </row>
+        <row r="190">
+          <cell r="C190">
+            <v>0.629</v>
+          </cell>
+        </row>
+        <row r="191">
+          <cell r="C191">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="192">
+          <cell r="C192">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="193">
+          <cell r="C193">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="194">
+          <cell r="C194">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="195">
+          <cell r="C195">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="196">
+          <cell r="C196">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="197">
+          <cell r="C197">
+            <v>1.5090000000000001</v>
+          </cell>
+        </row>
+        <row r="198">
+          <cell r="C198">
+            <v>0.72100000000000009</v>
+          </cell>
+        </row>
+        <row r="199">
+          <cell r="C199">
+            <v>0.6080000000000001</v>
+          </cell>
+        </row>
+        <row r="200">
+          <cell r="C200">
+            <v>0.113</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="C201">
+            <v>0.253</v>
+          </cell>
+        </row>
+        <row r="202">
+          <cell r="C202">
+            <v>20.356000000000002</v>
+          </cell>
+        </row>
+        <row r="203">
+          <cell r="C203">
+            <v>11.486000000000001</v>
+          </cell>
+        </row>
+        <row r="204">
+          <cell r="C204">
+            <v>9.7769999999999992</v>
+          </cell>
+        </row>
+        <row r="205">
+          <cell r="C205">
+            <v>1.7090000000000001</v>
+          </cell>
+        </row>
+        <row r="206">
+          <cell r="C206">
+            <v>7.492</v>
+          </cell>
+        </row>
+        <row r="207">
+          <cell r="C207">
+            <v>6.2510000000000003</v>
+          </cell>
+        </row>
+        <row r="208">
+          <cell r="C208">
+            <v>1.2409999999999999</v>
+          </cell>
+        </row>
+        <row r="209">
+          <cell r="C209">
+            <v>1.3779999999999999</v>
+          </cell>
+        </row>
+        <row r="210">
+          <cell r="C210">
+            <v>5.9039999999999999</v>
+          </cell>
+        </row>
+        <row r="211">
+          <cell r="C211">
+            <v>0.56000000000000005</v>
+          </cell>
+        </row>
+        <row r="212">
+          <cell r="C212">
+            <v>0.89500000000000002</v>
+          </cell>
+        </row>
+        <row r="213">
+          <cell r="C213">
+            <v>1.88</v>
+          </cell>
+        </row>
+        <row r="214">
+          <cell r="C214">
+            <v>1.7000000000000001E-2</v>
+          </cell>
+        </row>
+        <row r="215">
+          <cell r="C215">
+            <v>1.9619999999999997</v>
+          </cell>
+        </row>
+        <row r="216">
+          <cell r="C216">
+            <v>0.23700000000000002</v>
+          </cell>
+        </row>
+        <row r="217">
+          <cell r="C217">
+            <v>0.35300000000000004</v>
+          </cell>
+        </row>
+        <row r="218">
+          <cell r="C218">
+            <v>7.4689999999999994</v>
+          </cell>
+        </row>
+        <row r="219">
+          <cell r="C219">
+            <v>3.3540000000000001</v>
+          </cell>
+        </row>
+        <row r="220">
+          <cell r="C220">
+            <v>4.1150000000000002</v>
+          </cell>
+        </row>
+        <row r="221">
+          <cell r="C221">
+            <v>2.7719999999999998</v>
+          </cell>
+        </row>
+        <row r="222">
+          <cell r="C222">
+            <v>0.60799999999999998</v>
+          </cell>
+        </row>
+        <row r="223">
+          <cell r="C223">
+            <v>0.13700000000000001</v>
+          </cell>
+        </row>
+        <row r="224">
+          <cell r="C224">
+            <v>2.0269999999999997</v>
+          </cell>
+        </row>
+        <row r="225">
+          <cell r="C225">
+            <v>2.5270000000000001</v>
+          </cell>
+        </row>
+        <row r="226">
+          <cell r="C226">
+            <v>2.2610000000000001</v>
+          </cell>
+        </row>
+        <row r="227">
+          <cell r="C227">
+            <v>0.26600000000000001</v>
+          </cell>
+        </row>
+        <row r="228">
+          <cell r="C228">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="229">
+          <cell r="C229">
+            <v>2.0219999999999998</v>
+          </cell>
+        </row>
+        <row r="230">
+          <cell r="C230">
+            <v>3.0889999999999995</v>
+          </cell>
+        </row>
+        <row r="231">
+          <cell r="C231">
+            <v>1.474</v>
+          </cell>
+        </row>
+        <row r="232">
+          <cell r="C232">
+            <v>0.63</v>
+          </cell>
+        </row>
+        <row r="233">
+          <cell r="C233">
+            <v>0.98499999999999999</v>
+          </cell>
+        </row>
+        <row r="237">
+          <cell r="A237">
+            <v>2020</v>
+          </cell>
+          <cell r="C237" t="str">
+            <v>Economic Category Total</v>
+          </cell>
+        </row>
+        <row r="243">
+          <cell r="C243" t="str">
+            <v>Mt CO2 equivalent</v>
+          </cell>
+        </row>
+        <row r="244">
+          <cell r="A244" t="str">
+            <v>Totala,b</v>
+          </cell>
+          <cell r="C244">
+            <v>60.158999999999999</v>
+          </cell>
+        </row>
+        <row r="245">
+          <cell r="A245" t="str">
+            <v>ECONOMIC CATEGORY</v>
+          </cell>
+          <cell r="C245">
+            <v>14.702</v>
+          </cell>
+        </row>
+        <row r="246">
+          <cell r="C246">
+            <v>14.154000000000002</v>
+          </cell>
+        </row>
+        <row r="247">
+          <cell r="C247">
+            <v>12.189000000000002</v>
+          </cell>
+        </row>
+        <row r="248">
+          <cell r="C248">
+            <v>0.45100000000000001</v>
+          </cell>
+        </row>
+        <row r="249">
+          <cell r="C249">
+            <v>0.45100000000000001</v>
+          </cell>
+        </row>
+        <row r="250">
+          <cell r="C250">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="251">
+          <cell r="C251">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="252">
+          <cell r="C252">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="253">
+          <cell r="C253">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="254">
+          <cell r="C254">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="255">
+          <cell r="C255">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="256">
+          <cell r="C256">
+            <v>1.5140000000000002</v>
+          </cell>
+        </row>
+        <row r="257">
+          <cell r="C257">
+            <v>0.54800000000000004</v>
+          </cell>
+        </row>
+        <row r="258">
+          <cell r="C258">
+            <v>0.43000000000000005</v>
+          </cell>
+        </row>
+        <row r="259">
+          <cell r="C259">
+            <v>0.11800000000000001</v>
+          </cell>
+        </row>
+        <row r="260">
+          <cell r="C260">
+            <v>0.24099999999999999</v>
+          </cell>
+        </row>
+        <row r="261">
+          <cell r="C261">
+            <v>20.407</v>
+          </cell>
+        </row>
+        <row r="262">
+          <cell r="C262">
+            <v>10.366</v>
+          </cell>
+        </row>
+        <row r="263">
+          <cell r="C263">
+            <v>9.125</v>
+          </cell>
+        </row>
+        <row r="264">
+          <cell r="C264">
+            <v>1.2409999999999999</v>
+          </cell>
+        </row>
+        <row r="265">
+          <cell r="C265">
+            <v>8.1020000000000003</v>
+          </cell>
+        </row>
+        <row r="266">
+          <cell r="C266">
+            <v>6.5839999999999996</v>
+          </cell>
+        </row>
+        <row r="267">
+          <cell r="C267">
+            <v>1.518</v>
+          </cell>
+        </row>
+        <row r="268">
+          <cell r="C268">
+            <v>1.9390000000000001</v>
+          </cell>
+        </row>
+        <row r="269">
+          <cell r="C269">
+            <v>5.6079999999999997</v>
+          </cell>
+        </row>
+        <row r="270">
+          <cell r="C270">
+            <v>0.82799999999999996</v>
+          </cell>
+        </row>
+        <row r="271">
+          <cell r="C271">
+            <v>1.1479999999999999</v>
+          </cell>
+        </row>
+        <row r="272">
+          <cell r="C272">
+            <v>2.069</v>
+          </cell>
+        </row>
+        <row r="273">
+          <cell r="C273">
+            <v>3.6999999999999998E-2</v>
+          </cell>
+        </row>
+        <row r="274">
+          <cell r="C274">
+            <v>1.145</v>
+          </cell>
+        </row>
+        <row r="275">
+          <cell r="C275">
+            <v>8.8999999999999996E-2</v>
+          </cell>
+        </row>
+        <row r="276">
+          <cell r="C276">
+            <v>0.29199999999999998</v>
+          </cell>
+        </row>
+        <row r="277">
+          <cell r="C277">
+            <v>8.8460000000000001</v>
+          </cell>
+        </row>
+        <row r="278">
+          <cell r="C278">
+            <v>4.1079999999999997</v>
+          </cell>
+        </row>
+        <row r="279">
+          <cell r="C279">
+            <v>4.7379999999999995</v>
+          </cell>
+        </row>
+        <row r="280">
+          <cell r="C280">
+            <v>3.0979999999999999</v>
+          </cell>
+        </row>
+        <row r="281">
+          <cell r="C281">
+            <v>0.82699999999999996</v>
+          </cell>
+        </row>
+        <row r="282">
+          <cell r="C282">
+            <v>0.184</v>
+          </cell>
+        </row>
+        <row r="283">
+          <cell r="C283">
+            <v>2.0870000000000002</v>
+          </cell>
+        </row>
+        <row r="284">
+          <cell r="C284">
+            <v>1.9000000000000001</v>
+          </cell>
+        </row>
+        <row r="285">
+          <cell r="C285">
+            <v>1.6120000000000001</v>
+          </cell>
+        </row>
+        <row r="286">
+          <cell r="C286">
+            <v>0.28799999999999998</v>
+          </cell>
+        </row>
+        <row r="287">
+          <cell r="C287">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="288">
+          <cell r="C288">
+            <v>2.1059999999999999</v>
+          </cell>
+        </row>
+        <row r="289">
+          <cell r="C289">
+            <v>3.2510000000000003</v>
+          </cell>
+        </row>
+        <row r="290">
+          <cell r="C290">
+            <v>1.5050000000000001</v>
+          </cell>
+        </row>
+        <row r="291">
+          <cell r="C291">
+            <v>0.64700000000000002</v>
+          </cell>
+        </row>
+        <row r="292">
+          <cell r="C292">
+            <v>1.099</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -655,21 +2029,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6A09D5-1C1C-4B2D-9A8F-67854D65FEFF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3205D073-7870-41DE-BAC6-25B2643D22BC}">
   <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -743,7 +2117,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -765,52 +2139,52 @@
       <c r="L3" t="s">
         <v>19</v>
       </c>
-      <c r="M3">
-        <f>[1]BC!E$103</f>
-        <v>1000000</v>
-      </c>
-      <c r="N3">
-        <f>[1]BC!F$103</f>
-        <v>1300000</v>
-      </c>
-      <c r="O3">
-        <f>[1]BC!G$103</f>
-        <v>700000</v>
-      </c>
-      <c r="P3">
-        <f>[1]BC!H$103</f>
-        <v>1000000</v>
-      </c>
-      <c r="Q3">
-        <f>[1]BC!I$103</f>
-        <v>1100000</v>
+      <c r="M3" cm="1">
+        <f t="array" aca="1" ref="M3" ca="1">INDEX([1]BC_2!$C$1:$C$293,_xlfn.XMATCH(M$2,[1]BC_2!$A$1:$A$293)+55)*10^6</f>
+        <v>968000.00000000012</v>
+      </c>
+      <c r="N3" cm="1">
+        <f t="array" aca="1" ref="N3" ca="1">INDEX([1]BC_2!$C$1:$C$293,_xlfn.XMATCH(N$2,[1]BC_2!$A$1:$A$293)+55)*10^6</f>
+        <v>1251000</v>
+      </c>
+      <c r="O3" cm="1">
+        <f t="array" aca="1" ref="O3" ca="1">INDEX([1]BC_2!$C$1:$C$293,_xlfn.XMATCH(O$2,[1]BC_2!$A$1:$A$293)+55)*10^6</f>
+        <v>722000</v>
+      </c>
+      <c r="P3" cm="1">
+        <f t="array" aca="1" ref="P3" ca="1">INDEX([1]BC_2!$C$1:$C$293,_xlfn.XMATCH(P$2,[1]BC_2!$A$1:$A$293)+55)*10^6</f>
+        <v>985000</v>
+      </c>
+      <c r="Q3" cm="1">
+        <f t="array" aca="1" ref="Q3" ca="1">INDEX([1]BC_2!$C$1:$C$293,_xlfn.XMATCH(Q$2,[1]BC_2!$A$1:$A$293)+55)*10^6</f>
+        <v>1099000</v>
       </c>
       <c r="R3">
-        <f>[1]BC!J$103</f>
-        <v>1100000</v>
+        <f ca="1">Q3</f>
+        <v>1099000</v>
       </c>
       <c r="S3">
-        <f>[1]BC!K$103</f>
-        <v>1100000</v>
+        <f t="shared" ref="S3:W3" ca="1" si="0">R3</f>
+        <v>1099000</v>
       </c>
       <c r="T3">
-        <f>[1]BC!L$103</f>
-        <v>1100000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1099000</v>
       </c>
       <c r="U3">
-        <f>[1]BC!M$103</f>
-        <v>1100000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1099000</v>
       </c>
       <c r="V3">
-        <f>[1]BC!N$103</f>
-        <v>1100000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1099000</v>
       </c>
       <c r="W3">
-        <f>[1]BC!O$103</f>
-        <v>1100000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1099000</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -830,7 +2204,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -850,7 +2224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -909,7 +2283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -968,7 +2342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1027,7 +2401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1086,7 +2460,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1145,7 +2519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1204,7 +2578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1263,7 +2637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1322,7 +2696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1381,7 +2755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1440,7 +2814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1499,7 +2873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1558,7 +2932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1617,7 +2991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1676,7 +3050,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1735,7 +3109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1794,7 +3168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1853,7 +3227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1912,7 +3286,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1971,7 +3345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2030,7 +3404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2056,47 +3430,47 @@
         <v>1</v>
       </c>
       <c r="N26">
-        <f>M26</f>
+        <f ca="1">M26</f>
         <v>1</v>
       </c>
       <c r="O26">
-        <f t="shared" ref="O26:W26" si="0">N26</f>
+        <f t="shared" ref="O26:W26" ca="1" si="1">N26</f>
         <v>1</v>
       </c>
       <c r="P26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="R26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="S26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="T26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="U26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="V26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="W26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -2119,7 +3493,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -2142,7 +3516,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2165,7 +3539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2194,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2223,47 +3597,47 @@
         <v>20</v>
       </c>
       <c r="N31">
-        <f t="shared" ref="N31:W32" si="1">M31</f>
+        <f t="shared" ref="N31:W32" ca="1" si="2">M31</f>
         <v>20</v>
       </c>
       <c r="O31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="P31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="R31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="S31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="T31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="U31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="V31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
       <c r="W31">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2286,57 +3660,57 @@
         <v>17</v>
       </c>
       <c r="J32" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="L32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M32">
-        <f>1/0.070235</f>
+        <f ca="1">1/0.070235</f>
         <v>14.237915569160673</v>
       </c>
       <c r="N32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="O32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="P32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="R32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="S32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="T32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="U32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="V32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
       <c r="W32">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>14.237915569160673</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -2353,13 +3727,13 @@
         <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -2376,7 +3750,7 @@
         <v>47</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G34" t="s">
         <v>50</v>
@@ -2388,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2405,7 +3779,7 @@
         <v>47</v>
       </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
         <v>52</v>
@@ -2417,47 +3791,47 @@
         <v>20</v>
       </c>
       <c r="N35">
-        <f t="shared" ref="N35:W36" si="2">M35</f>
+        <f t="shared" ref="N35:W36" ca="1" si="3">M35</f>
         <v>20</v>
       </c>
       <c r="O35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="P35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="R35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="S35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="T35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="U35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="V35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
       <c r="W35">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -2474,7 +3848,7 @@
         <v>47</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G36" t="s">
         <v>17</v>
@@ -2483,50 +3857,50 @@
         <v>31</v>
       </c>
       <c r="L36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M36">
-        <f>1/0.070235</f>
+        <f ca="1">1/0.070235</f>
         <v>14.237915569160673</v>
       </c>
       <c r="N36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="O36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="P36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="R36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="S36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="T36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="U36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="V36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
       <c r="W36">
-        <f t="shared" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>14.237915569160673</v>
       </c>
     </row>

</xml_diff>